<commit_message>
ENH: Use new xlsx styling for dragNdrop conditions file
</commit_message>
<xml_diff>
--- a/psychopy/demos/builder/Experiments/dragAndDrop/conditions.xlsx
+++ b/psychopy/demos/builder/Experiments/dragAndDrop/conditions.xlsx
@@ -1,23 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Throwaway\PsychoPy3 Demos\Experiments\dragAndDrop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{744D70C6-7892-4BF2-A4DF-238702076018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="34050" yWindow="1185" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Work</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t xml:space="preserve">Name
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>A variable with this name will be created in PsychoPy, its value at any given time will be one of the cells below.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{E5458DB3-6A1D-4BE3-8E91-52D53E0F1609}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t xml:space="preserve">Values
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>Each iteration of this loop, a different one of these values will be chosen. This will be the value of the variable named above.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
   <si>
@@ -63,22 +140,22 @@
     <t>a9</t>
   </si>
   <si>
-    <t>white.png</t>
-  </si>
-  <si>
-    <t>black.png</t>
+    <t>design_41.png</t>
+  </si>
+  <si>
+    <t>whitePiece</t>
+  </si>
+  <si>
+    <t>blackPiece</t>
+  </si>
+  <si>
+    <t>design_42.png</t>
+  </si>
+  <si>
+    <t>design_43.png</t>
   </si>
   <si>
     <t>design_91.png</t>
-  </si>
-  <si>
-    <t>design_41.png</t>
-  </si>
-  <si>
-    <t>design_42.png</t>
-  </si>
-  <si>
-    <t>design_43.png</t>
   </si>
   <si>
     <t>design_92.png</t>
@@ -90,8 +167,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,13 +176,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2545B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,15 +226,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF2545B"/>
+      <color rgb="FF66666E"/>
+      <color rgb="FF02A9EA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -157,7 +276,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -169,7 +288,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -216,6 +335,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -251,6 +387,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,282 +555,286 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="1"/>
+    <col min="4" max="16384" width="20.7109375" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>300</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3">
         <v>300</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3">
         <v>200</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="3">
         <v>4</v>
       </c>
-      <c r="E2">
-        <f>IF(D2=4,2,3)</f>
+      <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4">
         <v>300</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4">
         <v>200</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="3">
         <v>4</v>
       </c>
-      <c r="E3">
-        <f>IF(D3=4,2,3)</f>
+      <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5">
         <v>300</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5">
         <v>200</v>
       </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <f>IF(D4=4,2,3)</f>
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
+      <c r="D5" s="3">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
         <v>300</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6">
         <v>200</v>
       </c>
-      <c r="D5">
+      <c r="D6" s="3">
         <v>9</v>
       </c>
-      <c r="E5">
+      <c r="E6" s="3">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" t="s">
-        <v>15</v>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1">
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
         <v>300</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7">
         <v>200</v>
       </c>
-      <c r="D6">
+      <c r="D7" s="3">
         <v>9</v>
       </c>
-      <c r="E6">
+      <c r="E7" s="3">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1">
-        <v>300</v>
-      </c>
-      <c r="C7" s="1">
-        <v>200</v>
-      </c>
-      <c r="D7">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" t="s">
-        <v>15</v>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>